<commit_message>
minor modifications for Cr
</commit_message>
<xml_diff>
--- a/ISO_Table_7_fc_values.xlsx
+++ b/ISO_Table_7_fc_values.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RishiSivakumar\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://atlanticbearing-my.sharepoint.com/personal/rishi_sivakumar_atlantic-bearing_com/Documents/Documents/GitHub/BearingManualAutomation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15287122-A6C6-446E-BCAE-9557D559D573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{15287122-A6C6-446E-BCAE-9557D559D573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F401942E-A63E-4D23-B83F-ADD3E38A157B}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -398,6 +398,10 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.81640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">

</xml_diff>